<commit_message>
Update Guess and Check Graphics
Signed-off-by: Will Hawkins <hawkinsw@obs.cr>
</commit_message>
<xml_diff>
--- a/data/guess_and_check_runtime_data.xlsx
+++ b/data/guess_and_check_runtime_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\whh8b\Code\Code\CPPTimes\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3F38D1B3-ED05-4E0F-87FB-42FE987BAE61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2616930-2C9F-4544-9304-6BDA796A0BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{60545851-F2E4-44E9-A99B-FE791E6C976D}"/>
   </bookViews>
@@ -92,6 +92,7 @@
     <mruColors>
       <color rgb="FFFF3333"/>
       <color rgb="FF5CC836"/>
+      <color rgb="FFF0FDFE"/>
     </mruColors>
   </colors>
   <extLst>
@@ -649,6 +650,387 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$125</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="124"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>490</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>560</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>570</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>580</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>590</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>610</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>620</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>630</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>660</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>670</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>680</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>690</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>710</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>730</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>740</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>760</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>770</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>790</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>810</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>820</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>830</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>840</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>860</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>870</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>880</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>890</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>910</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>920</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>930</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>940</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>950</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>960</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>970</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>990</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>1010</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>1020</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>1030</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>1040</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>1060</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>1070</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>1080</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>1090</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>1110</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>1120</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>1130</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>1140</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>1150</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>1160</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>1170</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>1180</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>1190</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>1210</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>1220</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>1230</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$C$2:$C$125</c:f>
@@ -1156,7 +1538,7 @@
         </c:txPr>
         <c:crossAx val="964702320"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
+        <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
@@ -1335,10 +1717,12 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="964720080"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1446,7 +1830,1807 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Number of Guesses Needed To Win</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Guesses (Naïve)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF3333"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$125</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="124"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>490</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>560</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>570</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>580</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>590</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>610</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>620</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>630</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>660</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>670</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>680</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>690</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>710</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>730</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>740</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>760</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>770</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>790</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>810</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>820</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>830</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>840</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>860</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>870</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>880</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>890</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>910</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>920</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>930</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>940</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>950</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>960</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>970</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>990</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>1010</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>1020</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>1030</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>1040</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>1060</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>1070</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>1080</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>1090</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>1110</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>1120</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>1130</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>1140</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>1150</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>1160</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>1170</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>1180</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>1190</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>1210</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>1220</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>1230</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$125</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="124"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>490</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>560</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>570</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>580</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>590</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>610</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>620</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>630</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>660</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>670</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>680</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>690</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>710</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>730</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>740</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>760</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>770</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>790</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>810</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>820</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>830</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>840</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>860</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>870</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>880</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>890</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>910</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>920</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>930</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>940</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>950</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>960</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>970</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>990</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>1010</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>1020</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>1030</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>1040</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>1060</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>1070</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>1080</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>1090</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>1110</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>1120</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>1130</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>1140</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>1150</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>1160</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>1170</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>1180</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>1190</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>1210</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>1220</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>1230</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F02D-4BDB-B5B0-B3750DA743F6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1320393551"/>
+        <c:axId val="1320392111"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Guesses (Blazin')</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="5CC836"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$125</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="124"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.3219280948873626</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.3219280948873626</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.9068905956085187</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.3219280948873626</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.6438561897747244</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.9068905956085187</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.1292830169449672</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.3219280948873617</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.4918530963296748</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.6438561897747253</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.7813597135246599</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.9068905956085187</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.0223678130284544</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.1292830169449664</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.2288186904958804</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7.3219280948873617</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7.4093909361377026</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7.4918530963296748</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7.5698556083309478</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7.6438561897747244</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>7.7142455176661224</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7.7813597135246608</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7.8454900509443757</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7.9068905956085187</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7.965784284662087</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8.0223678130284544</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8.0768155970508317</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>8.1292830169449655</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>8.1799090900149345</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8.2288186904958813</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8.2761244052742384</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8.3219280948873617</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8.366322214245816</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8.4093909361377026</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>8.451211111832329</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>8.4918530963296757</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>8.5313814605163127</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>8.5698556083309487</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>8.6073303137496104</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>8.6438561897747253</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>8.6794800995054473</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>8.7142455176661233</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>8.7481928495894596</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>8.7813597135246599</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>8.8137811912170374</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>8.8454900509443757</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>8.8765169465649993</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>8.9068905956085196</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>8.936637939002571</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>8.965784284662087</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>8.9943534368588587</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>9.0223678130284544</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>9.0498485494505623</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>9.0768155970508317</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>9.1032878084120217</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>9.1292830169449672</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>9.1548181090521048</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>9.1799090900149345</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>9.2045711442492042</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>9.2288186904958813</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>9.2526654324502502</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>9.2761244052742384</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>9.2992080183872794</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>9.3219280948873617</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>9.3442959079158179</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>9.366322214245816</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>9.3880172853451356</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>9.4093909361377008</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>9.4304525516655318</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>9.451211111832329</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>9.4716752143920449</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>9.4918530963296757</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>9.5117526537673793</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>9.5313814605163127</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>9.5507467853832431</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>9.5698556083309487</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>9.5887146355822637</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>9.6073303137496104</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>9.6257088430644657</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>9.6438561897747253</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>9.6617780977719878</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>9.6794800995054455</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>9.6969675262342871</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>9.7142455176661233</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>9.7313190310250643</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>9.7481928495894596</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>9.7648715907360906</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>9.7813597135246599</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>9.7976615258537603</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>9.8137811912170374</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>9.8297227350860581</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>9.8454900509443757</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>9.8610869059953927</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>9.8765169465650011</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>9.8917837032183105</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>9.9068905956085196</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>9.9218409370744904</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>9.936637939002571</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>9.9512847149669721</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>9.965784284662087</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>9.9801395776391573</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>9.9943534368588587</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>10.008428622070582</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>10.022367813028454</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>10.036173612553485</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>10.049848549450562</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>10.06339508128851</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>10.076815597050832</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>10.090112419664289</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>10.103287808412022</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>10.116343961237469</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>10.129283016944967</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>10.14210705730255</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>10.154818109052105</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>10.167418145831739</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>10.179909090014934</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>10.192292814470768</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>10.204571144249204</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>10.216745858195306</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>10.228818690495881</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>10.240791332161956</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>10.25266543245025</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>10.264442600226602</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F02D-4BDB-B5B0-B3750DA743F6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="27031599"/>
+        <c:axId val="199943535"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1320393551"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Possible Secret Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Choices</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1320392111"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1320392111"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Guesses (Naive method)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1320393551"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="199943535"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of Guesses (Binary method)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="27031599"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="27031599"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="199943535"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.603582239720035"/>
+          <c:y val="0.52835593467483233"/>
+          <c:w val="0.19826594200332825"/>
+          <c:h val="0.11015987558863964"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill>
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:srgbClr val="F0FDFE"/>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="tx2">
+            <a:lumMod val="10000"/>
+            <a:lumOff val="90000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:lin ang="5400000" scaled="1"/>
+    </a:gradFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2002,6 +4186,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -2035,6 +4735,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>240506</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{028B7AC5-2818-1512-1EE0-68DCBF86B41B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2106,6 +4842,327 @@
       <cdr:txBody>
         <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip"/>
         <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.00823</cdr:x>
+      <cdr:y>0.01214</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.05837</cdr:x>
+      <cdr:y>0.10325</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="Arrow: Right 2">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{021BCE25-A893-603B-9A50-4386D6DA8348}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="3784807">
+          <a:off x="14872" y="86728"/>
+          <a:ext cx="381450" cy="309593"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:srgbClr val="FF3333"/>
+        </a:solidFill>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </cdr:style>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.82746</cdr:x>
+      <cdr:y>0.10241</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.88016</cdr:x>
+      <cdr:y>0.20044</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="Arrow: Right 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{021BCE25-A893-603B-9A50-4386D6DA8348}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="3784807">
+          <a:off x="4824998" y="434390"/>
+          <a:ext cx="381450" cy="309593"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:srgbClr val="FF3333"/>
+        </a:solidFill>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </cdr:style>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:endParaRPr lang="en-US"/>
         </a:p>
@@ -2434,8 +5491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0598E2B1-40A3-4105-8D47-CBFE4AD89ACA}">
   <dimension ref="A1:C125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="N116" sqref="N116"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>